<commit_message>
Added columns in testdatasheet
</commit_message>
<xml_diff>
--- a/src/main/resources/testdatasheet.xlsx
+++ b/src/main/resources/testdatasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\workspace\PageObjectModelFramework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101DD090-92C2-49B0-A7D3-06743E3D1424}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22B3399-0BF7-43E7-8484-A5BBA37476CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="2" xr2:uid="{896CB679-BE82-4FC8-8EDB-A9B4BE5E2C6E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{896CB679-BE82-4FC8-8EDB-A9B4BE5E2C6E}"/>
   </bookViews>
   <sheets>
     <sheet name="testCasesMode" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>firstname</t>
   </si>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>SAG*@dem01234</t>
-  </si>
-  <si>
-    <t>nivakalita744@gmail.com</t>
-  </si>
-  <si>
-    <t>kalitaniva@1234</t>
   </si>
   <si>
     <t>Nayan Jyoti</t>
@@ -467,7 +461,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -475,7 +469,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -490,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4CBD2D-FEC9-40B1-8A07-6D604C5C9F41}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -520,26 +514,17 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{3A21478A-4173-453A-9C83-150D81FF21FD}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{4EA28CC2-D542-49D8-82B8-A6F9310F3E1E}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{7A0B2EDC-ACBB-439B-B5DF-0D88223B53E3}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{1A503EB4-C712-44B9-AD14-07B88235FFD9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -549,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748A6CE1-C271-4E7B-84BD-0F21CDDF69E6}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -571,15 +556,15 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>

</xml_diff>